<commit_message>
data: update testing_data.xlsx, remove Food Name and Nutrient Name columns from foods_nutrients
</commit_message>
<xml_diff>
--- a/test_mip_template/data/testing_data.xlsx
+++ b/test_mip_template/data/testing_data.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="41">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -535,7 +535,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="13.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="3" width="14.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="13.6"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="12.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="12.37"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3797,19 +3797,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E37"/>
+  <dimension ref="A1:C37"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H11" activeCellId="0" sqref="H11"/>
+      <selection pane="topLeft" activeCell="G7" activeCellId="0" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.16015625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="8.61"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="12.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="12.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="15.48"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="8" width="9.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="8" width="9.6"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3819,13 +3817,7 @@
       <c r="B1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="E1" s="9" t="s">
+      <c r="C1" s="9" t="s">
         <v>40</v>
       </c>
     </row>
@@ -3836,13 +3828,7 @@
       <c r="B2" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E2" s="8" t="n">
+      <c r="C2" s="8" t="n">
         <v>410</v>
       </c>
     </row>
@@ -3853,13 +3839,7 @@
       <c r="B3" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E3" s="8" t="n">
+      <c r="C3" s="8" t="n">
         <v>420</v>
       </c>
     </row>
@@ -3870,13 +3850,7 @@
       <c r="B4" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E4" s="8" t="n">
+      <c r="C4" s="8" t="n">
         <v>560</v>
       </c>
     </row>
@@ -3887,13 +3861,7 @@
       <c r="B5" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E5" s="8" t="n">
+      <c r="C5" s="8" t="n">
         <v>380</v>
       </c>
     </row>
@@ -3904,13 +3872,7 @@
       <c r="B6" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E6" s="8" t="n">
+      <c r="C6" s="8" t="n">
         <v>320</v>
       </c>
     </row>
@@ -3921,13 +3883,7 @@
       <c r="B7" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E7" s="8" t="n">
+      <c r="C7" s="8" t="n">
         <v>320</v>
       </c>
     </row>
@@ -3938,13 +3894,7 @@
       <c r="B8" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E8" s="8" t="n">
+      <c r="C8" s="8" t="n">
         <v>320</v>
       </c>
     </row>
@@ -3955,13 +3905,7 @@
       <c r="B9" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E9" s="8" t="n">
+      <c r="C9" s="8" t="n">
         <v>100</v>
       </c>
     </row>
@@ -3972,13 +3916,7 @@
       <c r="B10" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E10" s="8" t="n">
+      <c r="C10" s="8" t="n">
         <v>330</v>
       </c>
     </row>
@@ -3989,13 +3927,7 @@
       <c r="B11" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E11" s="8" t="n">
+      <c r="C11" s="8" t="n">
         <v>24</v>
       </c>
     </row>
@@ -4006,13 +3938,7 @@
       <c r="B12" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E12" s="8" t="n">
+      <c r="C12" s="8" t="n">
         <v>32</v>
       </c>
     </row>
@@ -4023,13 +3949,7 @@
       <c r="B13" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E13" s="8" t="n">
+      <c r="C13" s="8" t="n">
         <v>20</v>
       </c>
     </row>
@@ -4040,13 +3960,7 @@
       <c r="B14" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C14" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E14" s="8" t="n">
+      <c r="C14" s="8" t="n">
         <v>4</v>
       </c>
     </row>
@@ -4057,13 +3971,7 @@
       <c r="B15" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C15" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E15" s="8" t="n">
+      <c r="C15" s="8" t="n">
         <v>12</v>
       </c>
     </row>
@@ -4074,13 +3982,7 @@
       <c r="B16" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C16" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E16" s="8" t="n">
+      <c r="C16" s="8" t="n">
         <v>15</v>
       </c>
     </row>
@@ -4091,13 +3993,7 @@
       <c r="B17" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C17" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E17" s="8" t="n">
+      <c r="C17" s="8" t="n">
         <v>31</v>
       </c>
     </row>
@@ -4108,13 +4004,7 @@
       <c r="B18" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C18" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E18" s="8" t="n">
+      <c r="C18" s="8" t="n">
         <v>8</v>
       </c>
     </row>
@@ -4125,13 +4015,7 @@
       <c r="B19" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C19" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E19" s="8" t="n">
+      <c r="C19" s="8" t="n">
         <v>8</v>
       </c>
     </row>
@@ -4142,13 +4026,7 @@
       <c r="B20" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C20" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E20" s="8" t="n">
+      <c r="C20" s="8" t="n">
         <v>26</v>
       </c>
     </row>
@@ -4159,13 +4037,7 @@
       <c r="B21" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C21" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E21" s="8" t="n">
+      <c r="C21" s="8" t="n">
         <v>10</v>
       </c>
     </row>
@@ -4176,13 +4048,7 @@
       <c r="B22" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C22" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E22" s="8" t="n">
+      <c r="C22" s="8" t="n">
         <v>32</v>
       </c>
     </row>
@@ -4193,13 +4059,7 @@
       <c r="B23" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C23" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E23" s="8" t="n">
+      <c r="C23" s="8" t="n">
         <v>19</v>
       </c>
     </row>
@@ -4210,13 +4070,7 @@
       <c r="B24" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C24" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E24" s="8" t="n">
+      <c r="C24" s="8" t="n">
         <v>10</v>
       </c>
     </row>
@@ -4227,13 +4081,7 @@
       <c r="B25" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C25" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E25" s="8" t="n">
+      <c r="C25" s="8" t="n">
         <v>12</v>
       </c>
     </row>
@@ -4244,13 +4092,7 @@
       <c r="B26" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C26" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E26" s="8" t="n">
+      <c r="C26" s="8" t="n">
         <v>12</v>
       </c>
     </row>
@@ -4261,13 +4103,7 @@
       <c r="B27" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C27" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E27" s="8" t="n">
+      <c r="C27" s="8" t="n">
         <v>2.5</v>
       </c>
     </row>
@@ -4278,13 +4114,7 @@
       <c r="B28" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C28" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E28" s="8" t="n">
+      <c r="C28" s="8" t="n">
         <v>10</v>
       </c>
     </row>
@@ -4295,13 +4125,7 @@
       <c r="B29" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C29" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="E29" s="8" t="n">
+      <c r="C29" s="8" t="n">
         <v>730</v>
       </c>
     </row>
@@ -4312,13 +4136,7 @@
       <c r="B30" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C30" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="E30" s="8" t="n">
+      <c r="C30" s="8" t="n">
         <v>1190</v>
       </c>
     </row>
@@ -4329,13 +4147,7 @@
       <c r="B31" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C31" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="E31" s="8" t="n">
+      <c r="C31" s="8" t="n">
         <v>1800</v>
       </c>
     </row>
@@ -4346,13 +4158,7 @@
       <c r="B32" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C32" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="E32" s="8" t="n">
+      <c r="C32" s="8" t="n">
         <v>270</v>
       </c>
     </row>
@@ -4363,13 +4169,7 @@
       <c r="B33" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C33" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="E33" s="8" t="n">
+      <c r="C33" s="8" t="n">
         <v>930</v>
       </c>
     </row>
@@ -4380,13 +4180,7 @@
       <c r="B34" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C34" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="E34" s="8" t="n">
+      <c r="C34" s="8" t="n">
         <v>820</v>
       </c>
     </row>
@@ -4397,13 +4191,7 @@
       <c r="B35" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C35" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="E35" s="8" t="n">
+      <c r="C35" s="8" t="n">
         <v>1230</v>
       </c>
     </row>
@@ -4414,13 +4202,7 @@
       <c r="B36" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C36" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="E36" s="8" t="n">
+      <c r="C36" s="8" t="n">
         <v>125</v>
       </c>
     </row>
@@ -4431,13 +4213,7 @@
       <c r="B37" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C37" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="E37" s="8" t="n">
+      <c r="C37" s="8" t="n">
         <v>180</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Revert "data: update testing_data.xlsx, remove Food Name and Nutrient Name columns from foods_nutrients"
This reverts commit ab70400de1e7d1f54f4c2c818c0bd5c5cf44d8ec.
</commit_message>
<xml_diff>
--- a/test_mip_template/data/testing_data.xlsx
+++ b/test_mip_template/data/testing_data.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="41">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -535,7 +535,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="13.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="3" width="14.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="13.6"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="12.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="12.37"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3797,17 +3797,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C37"/>
+  <dimension ref="A1:E37"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G7" activeCellId="0" sqref="G7"/>
+      <selection pane="topLeft" activeCell="H11" activeCellId="0" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.16015625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="8.61"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="12.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="8" width="9.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="12.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="15.48"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="8" width="9.6"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3817,7 +3819,13 @@
       <c r="B1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" s="9" t="s">
         <v>40</v>
       </c>
     </row>
@@ -3828,7 +3836,13 @@
       <c r="B2" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C2" s="8" t="n">
+      <c r="C2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E2" s="8" t="n">
         <v>410</v>
       </c>
     </row>
@@ -3839,7 +3853,13 @@
       <c r="B3" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C3" s="8" t="n">
+      <c r="C3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E3" s="8" t="n">
         <v>420</v>
       </c>
     </row>
@@ -3850,7 +3870,13 @@
       <c r="B4" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C4" s="8" t="n">
+      <c r="C4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E4" s="8" t="n">
         <v>560</v>
       </c>
     </row>
@@ -3861,7 +3887,13 @@
       <c r="B5" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C5" s="8" t="n">
+      <c r="C5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E5" s="8" t="n">
         <v>380</v>
       </c>
     </row>
@@ -3872,7 +3904,13 @@
       <c r="B6" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C6" s="8" t="n">
+      <c r="C6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E6" s="8" t="n">
         <v>320</v>
       </c>
     </row>
@@ -3883,7 +3921,13 @@
       <c r="B7" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C7" s="8" t="n">
+      <c r="C7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E7" s="8" t="n">
         <v>320</v>
       </c>
     </row>
@@ -3894,7 +3938,13 @@
       <c r="B8" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C8" s="8" t="n">
+      <c r="C8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E8" s="8" t="n">
         <v>320</v>
       </c>
     </row>
@@ -3905,7 +3955,13 @@
       <c r="B9" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C9" s="8" t="n">
+      <c r="C9" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E9" s="8" t="n">
         <v>100</v>
       </c>
     </row>
@@ -3916,7 +3972,13 @@
       <c r="B10" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C10" s="8" t="n">
+      <c r="C10" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E10" s="8" t="n">
         <v>330</v>
       </c>
     </row>
@@ -3927,7 +3989,13 @@
       <c r="B11" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C11" s="8" t="n">
+      <c r="C11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E11" s="8" t="n">
         <v>24</v>
       </c>
     </row>
@@ -3938,7 +4006,13 @@
       <c r="B12" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C12" s="8" t="n">
+      <c r="C12" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E12" s="8" t="n">
         <v>32</v>
       </c>
     </row>
@@ -3949,7 +4023,13 @@
       <c r="B13" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C13" s="8" t="n">
+      <c r="C13" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E13" s="8" t="n">
         <v>20</v>
       </c>
     </row>
@@ -3960,7 +4040,13 @@
       <c r="B14" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C14" s="8" t="n">
+      <c r="C14" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E14" s="8" t="n">
         <v>4</v>
       </c>
     </row>
@@ -3971,7 +4057,13 @@
       <c r="B15" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C15" s="8" t="n">
+      <c r="C15" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E15" s="8" t="n">
         <v>12</v>
       </c>
     </row>
@@ -3982,7 +4074,13 @@
       <c r="B16" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C16" s="8" t="n">
+      <c r="C16" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E16" s="8" t="n">
         <v>15</v>
       </c>
     </row>
@@ -3993,7 +4091,13 @@
       <c r="B17" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C17" s="8" t="n">
+      <c r="C17" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E17" s="8" t="n">
         <v>31</v>
       </c>
     </row>
@@ -4004,7 +4108,13 @@
       <c r="B18" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C18" s="8" t="n">
+      <c r="C18" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E18" s="8" t="n">
         <v>8</v>
       </c>
     </row>
@@ -4015,7 +4125,13 @@
       <c r="B19" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C19" s="8" t="n">
+      <c r="C19" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E19" s="8" t="n">
         <v>8</v>
       </c>
     </row>
@@ -4026,7 +4142,13 @@
       <c r="B20" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C20" s="8" t="n">
+      <c r="C20" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E20" s="8" t="n">
         <v>26</v>
       </c>
     </row>
@@ -4037,7 +4159,13 @@
       <c r="B21" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C21" s="8" t="n">
+      <c r="C21" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E21" s="8" t="n">
         <v>10</v>
       </c>
     </row>
@@ -4048,7 +4176,13 @@
       <c r="B22" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C22" s="8" t="n">
+      <c r="C22" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E22" s="8" t="n">
         <v>32</v>
       </c>
     </row>
@@ -4059,7 +4193,13 @@
       <c r="B23" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C23" s="8" t="n">
+      <c r="C23" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E23" s="8" t="n">
         <v>19</v>
       </c>
     </row>
@@ -4070,7 +4210,13 @@
       <c r="B24" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C24" s="8" t="n">
+      <c r="C24" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E24" s="8" t="n">
         <v>10</v>
       </c>
     </row>
@@ -4081,7 +4227,13 @@
       <c r="B25" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C25" s="8" t="n">
+      <c r="C25" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E25" s="8" t="n">
         <v>12</v>
       </c>
     </row>
@@ -4092,7 +4244,13 @@
       <c r="B26" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C26" s="8" t="n">
+      <c r="C26" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E26" s="8" t="n">
         <v>12</v>
       </c>
     </row>
@@ -4103,7 +4261,13 @@
       <c r="B27" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C27" s="8" t="n">
+      <c r="C27" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E27" s="8" t="n">
         <v>2.5</v>
       </c>
     </row>
@@ -4114,7 +4278,13 @@
       <c r="B28" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C28" s="8" t="n">
+      <c r="C28" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E28" s="8" t="n">
         <v>10</v>
       </c>
     </row>
@@ -4125,7 +4295,13 @@
       <c r="B29" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C29" s="8" t="n">
+      <c r="C29" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E29" s="8" t="n">
         <v>730</v>
       </c>
     </row>
@@ -4136,7 +4312,13 @@
       <c r="B30" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C30" s="8" t="n">
+      <c r="C30" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E30" s="8" t="n">
         <v>1190</v>
       </c>
     </row>
@@ -4147,7 +4329,13 @@
       <c r="B31" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C31" s="8" t="n">
+      <c r="C31" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E31" s="8" t="n">
         <v>1800</v>
       </c>
     </row>
@@ -4158,7 +4346,13 @@
       <c r="B32" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C32" s="8" t="n">
+      <c r="C32" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E32" s="8" t="n">
         <v>270</v>
       </c>
     </row>
@@ -4169,7 +4363,13 @@
       <c r="B33" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C33" s="8" t="n">
+      <c r="C33" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E33" s="8" t="n">
         <v>930</v>
       </c>
     </row>
@@ -4180,7 +4380,13 @@
       <c r="B34" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C34" s="8" t="n">
+      <c r="C34" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E34" s="8" t="n">
         <v>820</v>
       </c>
     </row>
@@ -4191,7 +4397,13 @@
       <c r="B35" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C35" s="8" t="n">
+      <c r="C35" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E35" s="8" t="n">
         <v>1230</v>
       </c>
     </row>
@@ -4202,7 +4414,13 @@
       <c r="B36" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C36" s="8" t="n">
+      <c r="C36" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E36" s="8" t="n">
         <v>125</v>
       </c>
     </row>
@@ -4213,7 +4431,13 @@
       <c r="B37" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C37" s="8" t="n">
+      <c r="C37" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E37" s="8" t="n">
         <v>180</v>
       </c>
     </row>

</xml_diff>